<commit_message>
add: se corrije un error en la documentacion del ISA
</commit_message>
<xml_diff>
--- a/ISA y microarquitectura/ISA_formal.xlsx
+++ b/ISA y microarquitectura/ISA_formal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\proyectogrupal1\ISA y microarquitectura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A63CA1-D0E6-41D9-8CCA-4C25588E607D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416CD2DF-5545-4C90-A2B3-28935DF55837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="80">
   <si>
     <t>cond</t>
   </si>
@@ -88,9 +88,6 @@
   </si>
   <si>
     <t>JEQ</t>
-  </si>
-  <si>
-    <t>29:28</t>
   </si>
   <si>
     <t>00</t>
@@ -715,25 +712,103 @@
     <xf numFmtId="0" fontId="12" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="49" fontId="12" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="12" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -757,89 +832,11 @@
     <xf numFmtId="0" fontId="11" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="12" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="14" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="13" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="14" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="14" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="14" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1171,8 +1168,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
   <dimension ref="A1:I46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
+    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1193,21 +1190,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="26" t="s">
-        <v>70</v>
-      </c>
-      <c r="C1" s="26"/>
-      <c r="D1" s="26"/>
-      <c r="E1" s="26"/>
-      <c r="F1" s="26"/>
-      <c r="G1" s="26"/>
-      <c r="H1" s="26"/>
+      <c r="B1" s="56" t="s">
+        <v>69</v>
+      </c>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
+      <c r="G1" s="56"/>
+      <c r="H1" s="56"/>
       <c r="I1" s="7"/>
     </row>
     <row r="2" spans="1:9" ht="10.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B3" s="44" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
@@ -1217,341 +1214,341 @@
       <c r="H3" s="44"/>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="56" t="s">
-        <v>49</v>
-      </c>
-      <c r="C4" s="57"/>
-      <c r="D4" s="58"/>
-      <c r="E4" s="62" t="s">
+      <c r="B4" s="29" t="s">
         <v>48</v>
       </c>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="64"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="38" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
+      <c r="H4" s="40"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="50" t="s">
+      <c r="B5" s="26" t="s">
+        <v>45</v>
+      </c>
+      <c r="C5" s="26" t="s">
         <v>46</v>
       </c>
-      <c r="C5" s="50" t="s">
+      <c r="D5" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="D5" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="E5" s="65"/>
-      <c r="F5" s="66"/>
-      <c r="G5" s="66"/>
-      <c r="H5" s="67"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="42"/>
+      <c r="G5" s="42"/>
+      <c r="H5" s="43"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="51" t="s">
+      <c r="B6" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="51" t="s">
+      <c r="C6" s="27" t="s">
+        <v>42</v>
+      </c>
+      <c r="D6" s="27" t="s">
+        <v>62</v>
+      </c>
+      <c r="E6" s="35" t="s">
+        <v>79</v>
+      </c>
+      <c r="F6" s="36"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="37"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A7" s="28" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C7" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D6" s="51" t="s">
-        <v>63</v>
-      </c>
-      <c r="E6" s="59" t="s">
-        <v>80</v>
-      </c>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="61"/>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="52" t="s">
+      <c r="D7" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="E7" s="32" t="s">
         <v>78</v>
       </c>
-      <c r="B7" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C7" s="12" t="s">
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="34"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="28" t="s">
+        <v>76</v>
+      </c>
+      <c r="B8" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" s="12" t="s">
         <v>44</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E7" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="F7" s="54"/>
-      <c r="G7" s="54"/>
-      <c r="H7" s="55"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="52" t="s">
-        <v>77</v>
-      </c>
-      <c r="B8" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>45</v>
-      </c>
       <c r="D8" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="53" t="s">
-        <v>79</v>
-      </c>
-      <c r="F8" s="54"/>
-      <c r="G8" s="54"/>
-      <c r="H8" s="55"/>
+        <v>31</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>78</v>
+      </c>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="34"/>
     </row>
     <row r="9" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="10" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B10" s="46" t="s">
-        <v>52</v>
-      </c>
-      <c r="C10" s="46"/>
-      <c r="D10" s="46"/>
-      <c r="E10" s="46"/>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46"/>
-      <c r="H10" s="46"/>
+      <c r="B10" s="48" t="s">
+        <v>51</v>
+      </c>
+      <c r="C10" s="48"/>
+      <c r="D10" s="48"/>
+      <c r="E10" s="48"/>
+      <c r="F10" s="48"/>
+      <c r="G10" s="48"/>
+      <c r="H10" s="48"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="40" t="s">
+      <c r="B11" s="49" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="49"/>
+      <c r="D11" s="49"/>
+      <c r="E11" s="49" t="s">
         <v>49</v>
       </c>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="40" t="s">
-        <v>50</v>
-      </c>
-      <c r="F11" s="40"/>
-      <c r="G11" s="40"/>
-      <c r="H11" s="38" t="s">
-        <v>48</v>
+      <c r="F11" s="49"/>
+      <c r="G11" s="49"/>
+      <c r="H11" s="64" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>47</v>
-      </c>
       <c r="D12" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="E12" s="8" t="s">
-        <v>38</v>
-      </c>
       <c r="F12" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="G12" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="8" t="s">
-        <v>56</v>
-      </c>
-      <c r="H12" s="39"/>
+      <c r="H12" s="65"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="9" t="s">
         <v>14</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E13" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="F13" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G13" s="9" t="s">
         <v>66</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H13" s="9" t="s">
         <v>67</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B14" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C14" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D14" s="12">
         <v>0</v>
       </c>
       <c r="E14" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F14" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G14" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B15" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B16" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D16" s="12">
         <v>0</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D17" s="12">
         <v>0</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B18" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D18" s="12">
         <v>0</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D19" s="12">
         <v>0</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F19" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D20" s="12">
         <v>0</v>
       </c>
       <c r="E20" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -1566,29 +1563,29 @@
     </row>
     <row r="22" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="13"/>
-      <c r="B22" s="43" t="s">
-        <v>51</v>
-      </c>
-      <c r="C22" s="43"/>
-      <c r="D22" s="43"/>
-      <c r="E22" s="43"/>
-      <c r="F22" s="43"/>
-      <c r="G22" s="43"/>
-      <c r="H22" s="43"/>
+      <c r="B22" s="51" t="s">
+        <v>50</v>
+      </c>
+      <c r="C22" s="51"/>
+      <c r="D22" s="51"/>
+      <c r="E22" s="51"/>
+      <c r="F22" s="51"/>
+      <c r="G22" s="51"/>
+      <c r="H22" s="51"/>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="13"/>
-      <c r="B23" s="47" t="s">
+      <c r="B23" s="50" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="50"/>
+      <c r="D23" s="50"/>
+      <c r="E23" s="46" t="s">
         <v>49</v>
       </c>
-      <c r="C23" s="47"/>
-      <c r="D23" s="47"/>
-      <c r="E23" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="F23" s="42"/>
-      <c r="G23" s="42"/>
-      <c r="H23" s="42"/>
+      <c r="F23" s="46"/>
+      <c r="G23" s="46"/>
+      <c r="H23" s="46"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
@@ -1596,21 +1593,21 @@
         <v>13</v>
       </c>
       <c r="C24" s="17" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D24" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E24" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="E24" s="17" t="s">
+      <c r="F24" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G24" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="F24" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="G24" s="42" t="s">
-        <v>39</v>
-      </c>
-      <c r="H24" s="42"/>
+      <c r="H24" s="46"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
@@ -1618,417 +1615,437 @@
         <v>14</v>
       </c>
       <c r="C25" s="18" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D25" s="18" t="s">
+        <v>60</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="G25" s="47" t="s">
         <v>61</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>66</v>
-      </c>
-      <c r="G25" s="45" t="s">
-        <v>62</v>
-      </c>
-      <c r="H25" s="45"/>
+      <c r="H25" s="47"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B26" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D26" s="12">
         <v>1</v>
       </c>
       <c r="E26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G26" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F26" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G26" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H26" s="30"/>
+      <c r="H26" s="45"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B27" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D27" s="12">
         <v>1</v>
       </c>
       <c r="E27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G27" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G27" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H27" s="30"/>
+      <c r="H27" s="45"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B28" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D28" s="12">
         <v>1</v>
       </c>
       <c r="E28" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G28" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H28" s="30"/>
+      <c r="H28" s="45"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B29" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D29" s="12">
         <v>1</v>
       </c>
       <c r="E29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G29" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G29" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H29" s="30"/>
+      <c r="H29" s="45"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B30" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D30" s="12">
         <v>1</v>
       </c>
       <c r="E30" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F30" s="11" t="s">
+        <v>58</v>
+      </c>
+      <c r="G30" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>59</v>
-      </c>
-      <c r="G30" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H30" s="30"/>
+      <c r="H30" s="45"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B31" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D31" s="12">
         <v>1</v>
       </c>
       <c r="E31" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F31" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G31" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F31" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G31" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H31" s="30"/>
+      <c r="H31" s="45"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B32" s="11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D32" s="12">
         <v>1</v>
       </c>
       <c r="E32" s="11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F32" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G32" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="G32" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H32" s="30"/>
+      <c r="H32" s="45"/>
     </row>
     <row r="34" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="33" t="s">
-        <v>40</v>
-      </c>
-      <c r="C34" s="33"/>
-      <c r="D34" s="33"/>
-      <c r="E34" s="33"/>
-      <c r="F34" s="33"/>
-      <c r="G34" s="33"/>
-      <c r="H34" s="33"/>
+      <c r="B34" s="59" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="59"/>
+      <c r="D34" s="59"/>
+      <c r="E34" s="59"/>
+      <c r="F34" s="59"/>
+      <c r="G34" s="59"/>
+      <c r="H34" s="59"/>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="32" t="s">
-        <v>49</v>
-      </c>
-      <c r="C35" s="32"/>
-      <c r="D35" s="32"/>
-      <c r="E35" s="32" t="s">
-        <v>54</v>
-      </c>
-      <c r="F35" s="32"/>
-      <c r="G35" s="32"/>
-      <c r="H35" s="32"/>
+      <c r="B35" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C35" s="53"/>
+      <c r="D35" s="53"/>
+      <c r="E35" s="53" t="s">
+        <v>53</v>
+      </c>
+      <c r="F35" s="53"/>
+      <c r="G35" s="53"/>
+      <c r="H35" s="53"/>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B36" s="20" t="s">
+        <v>45</v>
+      </c>
+      <c r="C36" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="D36" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="D36" s="20" t="s">
-        <v>48</v>
-      </c>
       <c r="E36" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="F36" s="20" t="s">
+        <v>54</v>
+      </c>
+      <c r="G36" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="F36" s="20" t="s">
-        <v>55</v>
-      </c>
-      <c r="G36" s="32" t="s">
-        <v>39</v>
-      </c>
-      <c r="H36" s="32"/>
+      <c r="H36" s="53"/>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B37" s="21" t="s">
         <v>14</v>
       </c>
       <c r="C37" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D37" s="21" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E37" s="21" t="s">
+        <v>64</v>
+      </c>
+      <c r="F37" s="21" t="s">
         <v>65</v>
       </c>
-      <c r="F37" s="21" t="s">
-        <v>66</v>
-      </c>
-      <c r="G37" s="41" t="s">
-        <v>62</v>
-      </c>
-      <c r="H37" s="41"/>
+      <c r="G37" s="54" t="s">
+        <v>61</v>
+      </c>
+      <c r="H37" s="54"/>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B38" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C38" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D38" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E38" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F38" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G38" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F38" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G38" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H38" s="30"/>
+      <c r="H38" s="45"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B39" s="11" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E39" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="G39" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="F39" s="12" t="s">
-        <v>75</v>
-      </c>
-      <c r="G39" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H39" s="30"/>
+      <c r="H39" s="45"/>
     </row>
     <row r="41" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="31" t="s">
+      <c r="B41" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="31"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="31"/>
-      <c r="G41" s="31"/>
-      <c r="H41" s="31"/>
+      <c r="C41" s="58"/>
+      <c r="D41" s="58"/>
+      <c r="E41" s="58"/>
+      <c r="F41" s="58"/>
+      <c r="G41" s="58"/>
+      <c r="H41" s="58"/>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="28" t="s">
-        <v>49</v>
-      </c>
-      <c r="C42" s="28"/>
-      <c r="D42" s="28"/>
-      <c r="E42" s="34" t="s">
+      <c r="B42" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="F42" s="35"/>
-      <c r="G42" s="28" t="s">
-        <v>53</v>
-      </c>
-      <c r="H42" s="28"/>
+      <c r="C42" s="55"/>
+      <c r="D42" s="55"/>
+      <c r="E42" s="60" t="s">
+        <v>47</v>
+      </c>
+      <c r="F42" s="61"/>
+      <c r="G42" s="55" t="s">
+        <v>52</v>
+      </c>
+      <c r="H42" s="55"/>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B43" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C43" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="D43" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="D43" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="E43" s="36"/>
-      <c r="F43" s="37"/>
-      <c r="G43" s="28" t="s">
-        <v>39</v>
-      </c>
-      <c r="H43" s="28"/>
+      <c r="E43" s="62"/>
+      <c r="F43" s="63"/>
+      <c r="G43" s="55" t="s">
+        <v>38</v>
+      </c>
+      <c r="H43" s="55"/>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B44" s="24" t="s">
         <v>14</v>
       </c>
       <c r="C44" s="24" t="s">
-        <v>17</v>
+        <v>42</v>
       </c>
       <c r="D44" s="24" t="s">
-        <v>4</v>
-      </c>
-      <c r="E44" s="29" t="s">
-        <v>64</v>
-      </c>
-      <c r="F44" s="29"/>
-      <c r="G44" s="29" t="s">
         <v>62</v>
       </c>
-      <c r="H44" s="29"/>
+      <c r="E44" s="57" t="s">
+        <v>63</v>
+      </c>
+      <c r="F44" s="57"/>
+      <c r="G44" s="57" t="s">
+        <v>61</v>
+      </c>
+      <c r="H44" s="57"/>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" s="25" t="s">
         <v>15</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C45" s="11" t="s">
-        <v>18</v>
+        <v>43</v>
       </c>
       <c r="D45" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E45" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F45" s="27"/>
-      <c r="G45" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H45" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="E45" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F45" s="52"/>
+      <c r="G45" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H45" s="45"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
         <v>16</v>
       </c>
       <c r="B46" s="11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>19</v>
+        <v>44</v>
       </c>
       <c r="D46" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="E46" s="27" t="s">
-        <v>60</v>
-      </c>
-      <c r="F46" s="27"/>
-      <c r="G46" s="30" t="s">
-        <v>76</v>
-      </c>
-      <c r="H46" s="30"/>
+        <v>31</v>
+      </c>
+      <c r="E46" s="52" t="s">
+        <v>59</v>
+      </c>
+      <c r="F46" s="52"/>
+      <c r="G46" s="45" t="s">
+        <v>75</v>
+      </c>
+      <c r="H46" s="45"/>
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="E6:H6"/>
-    <mergeCell ref="E4:H5"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="G43:H43"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G42:H42"/>
+    <mergeCell ref="G45:H45"/>
+    <mergeCell ref="B41:H41"/>
+    <mergeCell ref="E35:H35"/>
+    <mergeCell ref="B34:H34"/>
+    <mergeCell ref="E44:F44"/>
+    <mergeCell ref="E42:F43"/>
+    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="E23:H23"/>
+    <mergeCell ref="B22:H22"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G36:H36"/>
+    <mergeCell ref="G46:H46"/>
     <mergeCell ref="B3:H3"/>
     <mergeCell ref="G29:H29"/>
     <mergeCell ref="G30:H30"/>
@@ -2040,31 +2057,11 @@
     <mergeCell ref="B10:H10"/>
     <mergeCell ref="E11:G11"/>
     <mergeCell ref="B23:D23"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="B1:H1"/>
-    <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E42:F43"/>
-    <mergeCell ref="H11:H12"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E6:H6"/>
+    <mergeCell ref="E4:H5"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2090,12 +2087,12 @@
   <sheetData>
     <row r="2" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="3" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A3" s="48" t="s">
+      <c r="A3" s="66" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="48"/>
-      <c r="C3" s="48"/>
-      <c r="D3" s="48"/>
+      <c r="B3" s="66"/>
+      <c r="C3" s="66"/>
+      <c r="D3" s="66"/>
     </row>
     <row r="4" spans="1:4" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="3" t="s">
@@ -2138,10 +2135,10 @@
       </c>
     </row>
     <row r="7" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="49" t="s">
+      <c r="B7" s="67" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="49"/>
+      <c r="C7" s="67"/>
       <c r="D7" s="5" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
add: first version of interpreter comunication
</commit_message>
<xml_diff>
--- a/ISA y microarquitectura/ISA_formal.xlsx
+++ b/ISA y microarquitectura/ISA_formal.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlo\OneDrive\Escritorio\proyectogrupal1\ISA y microarquitectura\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{416CD2DF-5545-4C90-A2B3-28935DF55837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{468B82D3-7401-4FB8-8265-498E997AA762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{5415A85A-6E18-4C2E-8E3D-011908CE6A7F}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="82">
   <si>
     <t>cond</t>
   </si>
@@ -210,9 +210,6 @@
     <t>11</t>
   </si>
   <si>
-    <t>Stall</t>
-  </si>
-  <si>
     <t>0000</t>
   </si>
   <si>
@@ -277,6 +274,15 @@
   </si>
   <si>
     <t>25:0</t>
+  </si>
+  <si>
+    <t>System</t>
+  </si>
+  <si>
+    <t>COM</t>
+  </si>
+  <si>
+    <t>29:28</t>
   </si>
 </sst>
 </file>
@@ -721,6 +727,27 @@
     <xf numFmtId="0" fontId="12" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -765,27 +792,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="14" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="12" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="11" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="10" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1166,10 +1172,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F98BBD8C-B9E8-4C66-8139-ABC2780EC3EF}">
-  <dimension ref="A1:I46"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="D45" sqref="D45"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1197,7 @@
   <sheetData>
     <row r="1" spans="1:9" ht="20.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="56" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C1" s="56"/>
       <c r="D1" s="56"/>
@@ -1203,28 +1209,28 @@
     </row>
     <row r="2" spans="1:9" ht="10.8" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B3" s="44" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="44"/>
-      <c r="D3" s="44"/>
-      <c r="E3" s="44"/>
-      <c r="F3" s="44"/>
-      <c r="G3" s="44"/>
-      <c r="H3" s="44"/>
+      <c r="B3" s="29" t="s">
+        <v>79</v>
+      </c>
+      <c r="C3" s="29"/>
+      <c r="D3" s="29"/>
+      <c r="E3" s="29"/>
+      <c r="F3" s="29"/>
+      <c r="G3" s="29"/>
+      <c r="H3" s="29"/>
     </row>
     <row r="4" spans="1:9" ht="14.4" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="29" t="s">
+      <c r="B4" s="36" t="s">
         <v>48</v>
       </c>
-      <c r="C4" s="30"/>
-      <c r="D4" s="31"/>
-      <c r="E4" s="38" t="s">
+      <c r="C4" s="37"/>
+      <c r="D4" s="38"/>
+      <c r="E4" s="45" t="s">
         <v>47</v>
       </c>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="40"/>
+      <c r="F4" s="46"/>
+      <c r="G4" s="46"/>
+      <c r="H4" s="47"/>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B5" s="26" t="s">
@@ -1236,830 +1242,852 @@
       <c r="D5" s="26" t="s">
         <v>47</v>
       </c>
-      <c r="E5" s="41"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="43"/>
+      <c r="E5" s="48"/>
+      <c r="F5" s="49"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="50"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B6" s="27" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="27" t="s">
-        <v>42</v>
+        <v>81</v>
       </c>
       <c r="D6" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="E6" s="35" t="s">
-        <v>79</v>
-      </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="36"/>
-      <c r="H6" s="37"/>
+        <v>4</v>
+      </c>
+      <c r="E6" s="42" t="s">
+        <v>78</v>
+      </c>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="44"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="28" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B7" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C7" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="F7" s="33"/>
-      <c r="G7" s="33"/>
-      <c r="H7" s="34"/>
+      <c r="C7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D7" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F7" s="40"/>
+      <c r="G7" s="40"/>
+      <c r="H7" s="41"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="28" t="s">
-        <v>76</v>
+        <v>80</v>
       </c>
       <c r="B8" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="12" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="32" t="s">
-        <v>78</v>
-      </c>
-      <c r="F8" s="33"/>
-      <c r="G8" s="33"/>
-      <c r="H8" s="34"/>
-    </row>
-    <row r="9" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
-      <c r="B10" s="48" t="s">
+      <c r="C8" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F8" s="40"/>
+      <c r="G8" s="40"/>
+      <c r="H8" s="41"/>
+    </row>
+    <row r="9" spans="1:9" ht="15.6" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="C9" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" s="39" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" s="40"/>
+      <c r="G9" s="40"/>
+      <c r="H9" s="41"/>
+    </row>
+    <row r="11" spans="1:9" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B11" s="33" t="s">
         <v>51</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B11" s="49" t="s">
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="34" t="s">
         <v>48</v>
       </c>
-      <c r="C11" s="49"/>
-      <c r="D11" s="49"/>
-      <c r="E11" s="49" t="s">
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="49"/>
-      <c r="G11" s="49"/>
-      <c r="H11" s="64" t="s">
+      <c r="F12" s="34"/>
+      <c r="G12" s="34"/>
+      <c r="H12" s="64" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B12" s="8" t="s">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="8" t="s">
+      <c r="C13" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="E12" s="8" t="s">
+      <c r="E13" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="8" t="s">
+      <c r="F13" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G12" s="8" t="s">
+      <c r="G13" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="H12" s="65"/>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="9" t="s">
+      <c r="H13" s="65"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C14" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="D13" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="E13" s="9" t="s">
+      <c r="D14" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="E14" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="F13" s="9" t="s">
+      <c r="G14" s="9" t="s">
         <v>65</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="H14" s="9" t="s">
         <v>66</v>
-      </c>
-      <c r="H13" s="9" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C14" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D14" s="12">
-        <v>0</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G14" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="H14" s="11" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="10" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B15" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D15" s="12">
         <v>0</v>
       </c>
       <c r="E15" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F15" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G15" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B16" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C16" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D16" s="12">
         <v>0</v>
       </c>
       <c r="E16" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F16" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G16" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="10" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B17" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C17" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D17" s="12">
         <v>0</v>
       </c>
       <c r="E17" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F17" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G17" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="10" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="B18" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C18" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D18" s="12">
         <v>0</v>
       </c>
       <c r="E18" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F18" s="11" t="s">
-        <v>58</v>
+        <v>73</v>
+      </c>
+      <c r="F18" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="G18" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="10" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B19" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C19" s="11" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="D19" s="12">
         <v>0</v>
       </c>
       <c r="E19" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F19" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
+      </c>
+      <c r="F19" s="11" t="s">
+        <v>57</v>
       </c>
       <c r="G19" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
-        <v>24</v>
+        <v>71</v>
       </c>
       <c r="B20" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C20" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D20" s="12">
         <v>0</v>
       </c>
-      <c r="E20" s="11" t="s">
-        <v>58</v>
+      <c r="E20" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="F20" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G20" s="12" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A21" s="13"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="13"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="13"/>
-      <c r="G21" s="13"/>
-      <c r="H21" s="16"/>
-    </row>
-    <row r="22" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
+        <v>24</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D21" s="12">
+        <v>0</v>
+      </c>
+      <c r="E21" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G21" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" ht="17.399999999999999" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="13"/>
-      <c r="B22" s="51" t="s">
+      <c r="B22" s="14"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="13"/>
+      <c r="E22" s="16"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="16"/>
+    </row>
+    <row r="23" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A23" s="13"/>
+      <c r="B23" s="51" t="s">
         <v>50</v>
       </c>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
-      <c r="G22" s="51"/>
-      <c r="H22" s="51"/>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="13"/>
-      <c r="B23" s="50" t="s">
-        <v>48</v>
-      </c>
-      <c r="C23" s="50"/>
-      <c r="D23" s="50"/>
-      <c r="E23" s="46" t="s">
-        <v>49</v>
-      </c>
-      <c r="F23" s="46"/>
-      <c r="G23" s="46"/>
-      <c r="H23" s="46"/>
+      <c r="C23" s="51"/>
+      <c r="D23" s="51"/>
+      <c r="E23" s="51"/>
+      <c r="F23" s="51"/>
+      <c r="G23" s="51"/>
+      <c r="H23" s="51"/>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="13"/>
-      <c r="B24" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="C24" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="D24" s="17" t="s">
-        <v>36</v>
-      </c>
-      <c r="E24" s="17" t="s">
-        <v>37</v>
-      </c>
-      <c r="F24" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="G24" s="46" t="s">
-        <v>38</v>
-      </c>
-      <c r="H24" s="46"/>
+      <c r="B24" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="C24" s="35"/>
+      <c r="D24" s="35"/>
+      <c r="E24" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="F24" s="31"/>
+      <c r="G24" s="31"/>
+      <c r="H24" s="31"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="13"/>
-      <c r="B25" s="18" t="s">
+      <c r="B25" s="17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" s="17" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>36</v>
+      </c>
+      <c r="E25" s="17" t="s">
+        <v>37</v>
+      </c>
+      <c r="F25" s="17" t="s">
+        <v>54</v>
+      </c>
+      <c r="G25" s="31" t="s">
+        <v>38</v>
+      </c>
+      <c r="H25" s="31"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A26" s="13"/>
+      <c r="B26" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="C25" s="18" t="s">
+      <c r="C26" s="18" t="s">
         <v>30</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D26" s="18" t="s">
+        <v>59</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="G26" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E25" s="18" t="s">
-        <v>64</v>
-      </c>
-      <c r="F25" s="18" t="s">
-        <v>65</v>
-      </c>
-      <c r="G25" s="47" t="s">
-        <v>61</v>
-      </c>
-      <c r="H25" s="47"/>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="19" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="11" t="s">
-        <v>18</v>
-      </c>
-      <c r="C26" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="12">
-        <v>1</v>
-      </c>
-      <c r="E26" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G26" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H26" s="45"/>
+      <c r="H26" s="32"/>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="19" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C27" s="11" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="D27" s="12">
         <v>1</v>
       </c>
       <c r="E27" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F27" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F27" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G27" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H27" s="45"/>
+      <c r="H27" s="30"/>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="19" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="12">
         <v>1</v>
       </c>
       <c r="E28" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F28" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G28" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F28" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G28" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H28" s="45"/>
+      <c r="H28" s="30"/>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="19" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="D29" s="12">
         <v>1</v>
       </c>
       <c r="E29" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F29" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G29" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F29" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G29" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H29" s="45"/>
+      <c r="H29" s="30"/>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="19" t="s">
-        <v>70</v>
+        <v>28</v>
       </c>
       <c r="B30" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D30" s="12">
         <v>1</v>
       </c>
       <c r="E30" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F30" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G30" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F30" s="11" t="s">
-        <v>58</v>
-      </c>
-      <c r="G30" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H30" s="45"/>
+      <c r="H30" s="30"/>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="19" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B31" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C31" s="11" t="s">
-        <v>71</v>
+        <v>35</v>
       </c>
       <c r="D31" s="12">
         <v>1</v>
       </c>
       <c r="E31" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F31" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="G31" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F31" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G31" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H31" s="45"/>
+      <c r="H31" s="30"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="19" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="B32" s="11" t="s">
         <v>18</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="D32" s="12">
         <v>1</v>
       </c>
-      <c r="E32" s="11" t="s">
-        <v>58</v>
+      <c r="E32" s="12" t="s">
+        <v>73</v>
       </c>
       <c r="F32" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G32" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="G32" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H32" s="45"/>
-    </row>
-    <row r="34" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="59" t="s">
+      <c r="H32" s="30"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A33" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>18</v>
+      </c>
+      <c r="C33" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="D33" s="12">
+        <v>1</v>
+      </c>
+      <c r="E33" s="11" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G33" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H33" s="30"/>
+    </row>
+    <row r="34" spans="1:8" ht="18" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B35" s="59" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="59"/>
-      <c r="D34" s="59"/>
-      <c r="E34" s="59"/>
-      <c r="F34" s="59"/>
-      <c r="G34" s="59"/>
-      <c r="H34" s="59"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B35" s="53" t="s">
+      <c r="C35" s="59"/>
+      <c r="D35" s="59"/>
+      <c r="E35" s="59"/>
+      <c r="F35" s="59"/>
+      <c r="G35" s="59"/>
+      <c r="H35" s="59"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B36" s="53" t="s">
         <v>48</v>
       </c>
-      <c r="C35" s="53"/>
-      <c r="D35" s="53"/>
-      <c r="E35" s="53" t="s">
+      <c r="C36" s="53"/>
+      <c r="D36" s="53"/>
+      <c r="E36" s="53" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="53"/>
-      <c r="G35" s="53"/>
-      <c r="H35" s="53"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B36" s="20" t="s">
+      <c r="F36" s="53"/>
+      <c r="G36" s="53"/>
+      <c r="H36" s="53"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B37" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C36" s="20" t="s">
+      <c r="C37" s="20" t="s">
         <v>46</v>
       </c>
-      <c r="D36" s="20" t="s">
+      <c r="D37" s="20" t="s">
         <v>47</v>
       </c>
-      <c r="E36" s="20" t="s">
+      <c r="E37" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="F36" s="20" t="s">
+      <c r="F37" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="G36" s="53" t="s">
+      <c r="G37" s="53" t="s">
         <v>38</v>
       </c>
-      <c r="H36" s="53"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B37" s="21" t="s">
+      <c r="H37" s="53"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B38" s="21" t="s">
         <v>14</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C38" s="21" t="s">
         <v>42</v>
       </c>
-      <c r="D37" s="21" t="s">
-        <v>62</v>
-      </c>
-      <c r="E37" s="21" t="s">
+      <c r="D38" s="21" t="s">
+        <v>61</v>
+      </c>
+      <c r="E38" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="F38" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="F37" s="21" t="s">
-        <v>65</v>
-      </c>
-      <c r="G37" s="54" t="s">
-        <v>61</v>
-      </c>
-      <c r="H37" s="54"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="11" t="s">
-        <v>19</v>
-      </c>
-      <c r="C38" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D38" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E38" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="F38" s="12" t="s">
-        <v>74</v>
-      </c>
-      <c r="G38" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H38" s="45"/>
+      <c r="G38" s="54" t="s">
+        <v>60</v>
+      </c>
+      <c r="H38" s="54"/>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="22" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B39" s="11" t="s">
         <v>19</v>
       </c>
       <c r="C39" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D39" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E39" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F39" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G39" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="F39" s="12" t="s">
+      <c r="H39" s="30"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A40" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="C40" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D40" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E40" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="F40" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="G40" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="G39" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H39" s="45"/>
-    </row>
-    <row r="41" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B41" s="58" t="s">
+      <c r="H40" s="30"/>
+    </row>
+    <row r="41" spans="1:8" ht="15.6" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="42" spans="1:8" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="B42" s="58" t="s">
         <v>12</v>
       </c>
-      <c r="C41" s="58"/>
-      <c r="D41" s="58"/>
-      <c r="E41" s="58"/>
-      <c r="F41" s="58"/>
-      <c r="G41" s="58"/>
-      <c r="H41" s="58"/>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B42" s="55" t="s">
+      <c r="C42" s="58"/>
+      <c r="D42" s="58"/>
+      <c r="E42" s="58"/>
+      <c r="F42" s="58"/>
+      <c r="G42" s="58"/>
+      <c r="H42" s="58"/>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B43" s="55" t="s">
         <v>48</v>
       </c>
-      <c r="C42" s="55"/>
-      <c r="D42" s="55"/>
-      <c r="E42" s="60" t="s">
+      <c r="C43" s="55"/>
+      <c r="D43" s="55"/>
+      <c r="E43" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="F42" s="61"/>
-      <c r="G42" s="55" t="s">
+      <c r="F43" s="61"/>
+      <c r="G43" s="55" t="s">
         <v>52</v>
       </c>
-      <c r="H42" s="55"/>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B43" s="23" t="s">
+      <c r="H43" s="55"/>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B44" s="23" t="s">
         <v>45</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C44" s="23" t="s">
         <v>46</v>
       </c>
-      <c r="D43" s="23" t="s">
+      <c r="D44" s="23" t="s">
         <v>47</v>
       </c>
-      <c r="E43" s="62"/>
-      <c r="F43" s="63"/>
-      <c r="G43" s="55" t="s">
+      <c r="E44" s="62"/>
+      <c r="F44" s="63"/>
+      <c r="G44" s="55" t="s">
         <v>38</v>
       </c>
-      <c r="H43" s="55"/>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="B44" s="24" t="s">
+      <c r="H44" s="55"/>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B45" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C44" s="24" t="s">
+      <c r="C45" s="24" t="s">
         <v>42</v>
       </c>
-      <c r="D44" s="24" t="s">
+      <c r="D45" s="24" t="s">
+        <v>61</v>
+      </c>
+      <c r="E45" s="57" t="s">
         <v>62</v>
       </c>
-      <c r="E44" s="57" t="s">
-        <v>63</v>
-      </c>
-      <c r="F44" s="57"/>
-      <c r="G44" s="57" t="s">
-        <v>61</v>
-      </c>
-      <c r="H44" s="57"/>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="25" t="s">
-        <v>15</v>
-      </c>
-      <c r="B45" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="C45" s="11" t="s">
-        <v>43</v>
-      </c>
-      <c r="D45" s="11" t="s">
-        <v>31</v>
-      </c>
-      <c r="E45" s="52" t="s">
-        <v>59</v>
-      </c>
-      <c r="F45" s="52"/>
-      <c r="G45" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H45" s="45"/>
+      <c r="F45" s="57"/>
+      <c r="G45" s="57" t="s">
+        <v>60</v>
+      </c>
+      <c r="H45" s="57"/>
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" s="25" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B46" s="11" t="s">
         <v>56</v>
       </c>
       <c r="C46" s="11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D46" s="11" t="s">
         <v>31</v>
       </c>
       <c r="E46" s="52" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F46" s="52"/>
-      <c r="G46" s="45" t="s">
-        <v>75</v>
-      </c>
-      <c r="H46" s="45"/>
+      <c r="G46" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H46" s="30"/>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A47" s="25" t="s">
+        <v>16</v>
+      </c>
+      <c r="B47" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="C47" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E47" s="52" t="s">
+        <v>58</v>
+      </c>
+      <c r="F47" s="52"/>
+      <c r="G47" s="30" t="s">
+        <v>74</v>
+      </c>
+      <c r="H47" s="30"/>
     </row>
   </sheetData>
-  <mergeCells count="41">
+  <mergeCells count="42">
+    <mergeCell ref="E8:H8"/>
     <mergeCell ref="B1:H1"/>
+    <mergeCell ref="G44:H44"/>
+    <mergeCell ref="G45:H45"/>
     <mergeCell ref="G43:H43"/>
-    <mergeCell ref="G44:H44"/>
-    <mergeCell ref="G42:H42"/>
-    <mergeCell ref="G45:H45"/>
-    <mergeCell ref="B41:H41"/>
-    <mergeCell ref="E35:H35"/>
-    <mergeCell ref="B34:H34"/>
-    <mergeCell ref="E44:F44"/>
-    <mergeCell ref="E42:F43"/>
-    <mergeCell ref="H11:H12"/>
+    <mergeCell ref="G46:H46"/>
+    <mergeCell ref="B42:H42"/>
+    <mergeCell ref="E36:H36"/>
+    <mergeCell ref="B35:H35"/>
     <mergeCell ref="E45:F45"/>
-    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="E43:F44"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="G33:H33"/>
     <mergeCell ref="G32:H32"/>
+    <mergeCell ref="E24:H24"/>
+    <mergeCell ref="B23:H23"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="G38:H38"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="G39:H39"/>
+    <mergeCell ref="G40:H40"/>
+    <mergeCell ref="G37:H37"/>
+    <mergeCell ref="G47:H47"/>
+    <mergeCell ref="B3:H3"/>
+    <mergeCell ref="G30:H30"/>
     <mergeCell ref="G31:H31"/>
-    <mergeCell ref="E23:H23"/>
-    <mergeCell ref="B22:H22"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="G37:H37"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="G38:H38"/>
-    <mergeCell ref="G39:H39"/>
-    <mergeCell ref="G36:H36"/>
-    <mergeCell ref="G46:H46"/>
-    <mergeCell ref="B3:H3"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="G24:H24"/>
     <mergeCell ref="G25:H25"/>
     <mergeCell ref="G26:H26"/>
     <mergeCell ref="G27:H27"/>
     <mergeCell ref="G28:H28"/>
-    <mergeCell ref="B10:H10"/>
-    <mergeCell ref="E11:G11"/>
-    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="E12:G12"/>
+    <mergeCell ref="B24:D24"/>
     <mergeCell ref="B4:D4"/>
     <mergeCell ref="E7:H7"/>
-    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="E9:H9"/>
     <mergeCell ref="E6:H6"/>
     <mergeCell ref="E4:H5"/>
   </mergeCells>
@@ -2067,7 +2095,7 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="E20" numberStoredAsText="1"/>
+    <ignoredError sqref="E21" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>

</xml_diff>